<commit_message>
feat: Generate G.T. label
</commit_message>
<xml_diff>
--- a/computer_vision/self_supervised_learning/colorization/quantized_ab_color_space.xlsx
+++ b/computer_vision/self_supervised_learning/colorization/quantized_ab_color_space.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jongbeomkim/Desktop/workspace/machine_learning/computer_vision/self_supervised_learning/colorization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B789021C-0373-4B25-B30F-2EEEC1237FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D72241-DA9D-3C41-A88A-1CEFB2937043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{BFD6A459-B4BC-48E0-825D-271C8EDF5EF1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="20980" xr2:uid="{BFD6A459-B4BC-48E0-825D-271C8EDF5EF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="23">
   <si>
     <t>-5 / 5</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -123,10 +120,6 @@
   </si>
   <si>
     <t>95 105</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>105 115</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -142,14 +135,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -318,7 +311,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -358,9 +351,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -376,7 +378,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -672,19 +674,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A257FEF6-234D-4011-B70F-BFAFA88C5EFA}">
-  <dimension ref="A1:X24"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+      <selection activeCell="W2" sqref="B2:W21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" style="1" customWidth="1"/>
     <col min="2" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
@@ -751,13 +753,10 @@
       <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
@@ -775,17 +774,26 @@
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="4"/>
-    </row>
-    <row r="3" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" s="4"/>
+    </row>
+    <row r="3" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -800,20 +808,35 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="7"/>
-    </row>
-    <row r="4" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="V3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="W3" s="7"/>
+    </row>
+    <row r="4" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
@@ -826,32 +849,41 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
+      <c r="M4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="R4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="W4" s="6"/>
-      <c r="X4" s="7"/>
-    </row>
-    <row r="5" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="W4" s="7"/>
+    </row>
+    <row r="5" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
@@ -862,40 +894,47 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
+      <c r="K5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="O5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="W5" s="6"/>
-      <c r="X5" s="7"/>
-    </row>
-    <row r="6" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="W5" s="7"/>
+    </row>
+    <row r="6" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
@@ -905,45 +944,52 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
+      <c r="J6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="M6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="W6" s="6"/>
-      <c r="X6" s="7"/>
-    </row>
-    <row r="7" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="W6" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
@@ -952,50 +998,55 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="I7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="K7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="W7" s="6"/>
-      <c r="X7" s="7"/>
-    </row>
-    <row r="8" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="W7" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
@@ -1003,55 +1054,58 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="H8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="J8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="W8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="X8" s="7"/>
-    </row>
-    <row r="9" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="W8" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
@@ -1059,971 +1113,812 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="I9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="W9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="X9" s="7"/>
-    </row>
-    <row r="10" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="W9" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="H10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="W10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="X10" s="7"/>
-    </row>
-    <row r="11" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="W10" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="H11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="W11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="X11" s="7"/>
-    </row>
-    <row r="12" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="W11" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="E12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="G12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U12" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="W12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="X12" s="7"/>
-    </row>
-    <row r="13" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="W12" s="7"/>
+    </row>
+    <row r="13" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="E13" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="F13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="W13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="X13" s="7"/>
-    </row>
-    <row r="14" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="W13" s="7"/>
+    </row>
+    <row r="14" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="D14" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="W14" s="6"/>
-      <c r="X14" s="7"/>
-    </row>
-    <row r="15" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="W14" s="7"/>
+    </row>
+    <row r="15" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="C15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="E15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V15" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="W15" s="6"/>
-      <c r="X15" s="7"/>
-    </row>
-    <row r="16" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="W15" s="7"/>
+    </row>
+    <row r="16" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
+      <c r="C16" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="D16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T16" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U16" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="V16" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="W16" s="6"/>
-      <c r="X16" s="7"/>
-    </row>
-    <row r="17" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="V16" s="6"/>
+      <c r="W16" s="7"/>
+    </row>
+    <row r="17" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="C17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T17" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U17" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="V17" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="W17" s="6"/>
-      <c r="X17" s="7"/>
-    </row>
-    <row r="18" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="V17" s="6"/>
+      <c r="W17" s="7"/>
+    </row>
+    <row r="18" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="C18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U18" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V18" s="6"/>
-      <c r="W18" s="6"/>
-      <c r="X18" s="7"/>
-    </row>
-    <row r="19" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W18" s="7"/>
+    </row>
+    <row r="19" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T19" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="U19" s="8" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="U19" s="6"/>
       <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="7"/>
-    </row>
-    <row r="20" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W19" s="7"/>
+    </row>
+    <row r="20" spans="1:23" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T20" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="U20" s="8" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="U20" s="6"/>
       <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="7"/>
-    </row>
-    <row r="21" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W20" s="7"/>
+    </row>
+    <row r="21" spans="1:23" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="R21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="S21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="T21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6"/>
-      <c r="W21" s="6"/>
-      <c r="X21" s="7"/>
-    </row>
-    <row r="22" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="R22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="S22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="T22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="U22" s="6"/>
-      <c r="V22" s="6"/>
-      <c r="W22" s="6"/>
-      <c r="X22" s="7"/>
-    </row>
-    <row r="23" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L23" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M23" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="6"/>
-      <c r="X23" s="7"/>
-    </row>
-    <row r="24" spans="1:24" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="12"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>